<commit_message>
REAL FINAL SUBMISSION FOR EXCEL FILE
</commit_message>
<xml_diff>
--- a/G6 TestCases.xlsx
+++ b/G6 TestCases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="88">
   <si>
     <t>Test Case Template</t>
   </si>
@@ -51,13 +51,13 @@
     <t>Test Executed By</t>
   </si>
   <si>
-    <t>UnitTest_1 (coder pov)</t>
+    <t>UnitTest_1</t>
   </si>
   <si>
     <t>a function or method</t>
   </si>
   <si>
-    <t>P</t>
+    <t>P1</t>
   </si>
   <si>
     <t>Viewing movie showtimes</t>
@@ -82,7 +82,13 @@
     <t>RogerD</t>
   </si>
   <si>
-    <t>FunctionalTest_1 (user's pov)</t>
+    <t>FunctionalTest_1</t>
+  </si>
+  <si>
+    <t>User Registration</t>
+  </si>
+  <si>
+    <t>P2</t>
   </si>
   <si>
     <t>Customer regristration (does the regristration actually register a user )</t>
@@ -103,6 +109,9 @@
   </si>
   <si>
     <t>SystemTest_1</t>
+  </si>
+  <si>
+    <t>User Signin</t>
   </si>
   <si>
     <t>Customer sign-in</t>
@@ -127,9 +136,6 @@
   </si>
   <si>
     <t>Ticket_Submission</t>
-  </si>
-  <si>
-    <t>P1</t>
   </si>
   <si>
     <t>Verify that when a user submits a ticket the customer service team receives it.</t>
@@ -406,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -428,9 +434,6 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -794,24 +797,26 @@
       <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="C4" s="7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>19</v>
@@ -838,26 +843,28 @@
     </row>
     <row r="5" ht="72.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="C5" s="7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>19</v>
@@ -884,34 +891,34 @@
     </row>
     <row r="6" ht="72.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>36</v>
+      <c r="D6" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="6"/>
@@ -932,34 +939,34 @@
     </row>
     <row r="7" ht="72.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="6"/>
@@ -980,34 +987,34 @@
     </row>
     <row r="8" ht="72.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="6"/>
@@ -1028,34 +1035,34 @@
     </row>
     <row r="9" ht="72.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="6"/>
@@ -1076,34 +1083,34 @@
     </row>
     <row r="10" ht="72.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="6"/>
@@ -1124,34 +1131,34 @@
     </row>
     <row r="11" ht="72.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="6"/>
@@ -1172,34 +1179,34 @@
     </row>
     <row r="12" ht="72.0" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="6"/>

</xml_diff>